<commit_message>
SW added bw roster & updated team captains
</commit_message>
<xml_diff>
--- a/secure/team-captains-list2019.xlsx
+++ b/secure/team-captains-list2019.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937C2B71-D718-4D28-8938-4F7E5D537CA4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC18D8A4-5D91-4702-8799-4681572A7EB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="2055" windowWidth="21600" windowHeight="11835" xr2:uid="{A3301E8E-CBA9-48DE-A787-1B2E0D3F0D20}"/>
+    <workbookView xWindow="2730" yWindow="1935" windowWidth="21540" windowHeight="14265" xr2:uid="{A3301E8E-CBA9-48DE-A787-1B2E0D3F0D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$52</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="164">
   <si>
     <t>Burnaby Mountain</t>
   </si>
@@ -43,78 +43,6 @@
     <t>skidvm59@gmail.com</t>
   </si>
   <si>
-    <t>Capilano</t>
-  </si>
-  <si>
-    <t>Marilyn Moscovitch</t>
-  </si>
-  <si>
-    <t>604-926-5260</t>
-  </si>
-  <si>
-    <t>marilynmoscovitch@gmail.com</t>
-  </si>
-  <si>
-    <t>Point Grey</t>
-  </si>
-  <si>
-    <t>Caddy Quong</t>
-  </si>
-  <si>
-    <t>604-736-7195</t>
-  </si>
-  <si>
-    <t>caddyquong@yahoo.com</t>
-  </si>
-  <si>
-    <t>Quilchena</t>
-  </si>
-  <si>
-    <t>Anita Ng</t>
-  </si>
-  <si>
-    <t>604-821-0016</t>
-  </si>
-  <si>
-    <t>Anitang66@hotmail.com</t>
-  </si>
-  <si>
-    <t>Richmond</t>
-  </si>
-  <si>
-    <t>Malee Rubinstein</t>
-  </si>
-  <si>
-    <t>604-803-6636</t>
-  </si>
-  <si>
-    <t>malee@r-tips.com</t>
-  </si>
-  <si>
-    <t>Seymour</t>
-  </si>
-  <si>
-    <t>Edna Dechant</t>
-  </si>
-  <si>
-    <t>604-563-2108</t>
-  </si>
-  <si>
-    <t>edna_d21@shaw.ca</t>
-  </si>
-  <si>
-    <t>Shaughnessy</t>
-  </si>
-  <si>
-    <t>Christina Wong</t>
-  </si>
-  <si>
-    <t>604-802-9468</t>
-  </si>
-  <si>
-    <t>chriskowong@telus.net</t>
-  </si>
-  <si>
     <t>University</t>
   </si>
   <si>
@@ -127,18 +55,6 @@
     <t>suenamgolf@gmail.com</t>
   </si>
   <si>
-    <t>Vancouver</t>
-  </si>
-  <si>
-    <t>Ashleigh Brown</t>
-  </si>
-  <si>
-    <t>604 346-6303</t>
-  </si>
-  <si>
-    <t>Ashleigh.brown@roberthalf.com</t>
-  </si>
-  <si>
     <t>Vancouver Chinese</t>
   </si>
   <si>
@@ -232,33 +148,6 @@
     <t>jkrug@telus.net</t>
   </si>
   <si>
-    <t>Shelagh Weatherill</t>
-  </si>
-  <si>
-    <t>604-261-9675</t>
-  </si>
-  <si>
-    <t>shelagh_weatherill@live.com</t>
-  </si>
-  <si>
-    <t>Susan Fugman</t>
-  </si>
-  <si>
-    <t>604-341-4344</t>
-  </si>
-  <si>
-    <t>sfugman@telus.net</t>
-  </si>
-  <si>
-    <t>Ruth Harris</t>
-  </si>
-  <si>
-    <t>604-803-5157</t>
-  </si>
-  <si>
-    <t>reharris@telus.net</t>
-  </si>
-  <si>
     <t>Squamish</t>
   </si>
   <si>
@@ -280,15 +169,6 @@
     <t>judydowler@telus.net</t>
   </si>
   <si>
-    <t>Terrie Levitt</t>
-  </si>
-  <si>
-    <t>604-836-7340</t>
-  </si>
-  <si>
-    <t>rialto8@telus.net</t>
-  </si>
-  <si>
     <t>Pauline Hui</t>
   </si>
   <si>
@@ -406,15 +286,6 @@
     <t>b_iwata@hotmail.com</t>
   </si>
   <si>
-    <t>Christine Dixon</t>
-  </si>
-  <si>
-    <t>604-261-6701</t>
-  </si>
-  <si>
-    <t>tindixon@gmail.com</t>
-  </si>
-  <si>
     <t>Sunshine Coast</t>
   </si>
   <si>
@@ -542,13 +413,121 @@
   </si>
   <si>
     <t>2019 Zone 4 &amp; Zone 3/4 Team Captains</t>
+  </si>
+  <si>
+    <t>Chilliwack</t>
+  </si>
+  <si>
+    <t>Fort Langley</t>
+  </si>
+  <si>
+    <t>Guildford</t>
+  </si>
+  <si>
+    <t>Ledgeview</t>
+  </si>
+  <si>
+    <t>Peace Portal</t>
+  </si>
+  <si>
+    <t>Surrey</t>
+  </si>
+  <si>
+    <t>Swan-e-set</t>
+  </si>
+  <si>
+    <t>McCleery</t>
+  </si>
+  <si>
+    <t>Sara MacFayden</t>
+  </si>
+  <si>
+    <t>604-607+5405</t>
+  </si>
+  <si>
+    <t>sarajanemac@gmail.com</t>
+  </si>
+  <si>
+    <t>Ingrid Bruhs</t>
+  </si>
+  <si>
+    <t>inggyb62@gmail.com</t>
+  </si>
+  <si>
+    <t>Kate Kim</t>
+  </si>
+  <si>
+    <t>604-374-6238</t>
+  </si>
+  <si>
+    <t>nanikim0811@gmail.com</t>
+  </si>
+  <si>
+    <t>Darlene Wenham</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-793-8116 </t>
+  </si>
+  <si>
+    <t>ddweden@gmail.com</t>
+  </si>
+  <si>
+    <t>Donna Larter</t>
+  </si>
+  <si>
+    <t>604-371-2995</t>
+  </si>
+  <si>
+    <t>bodolar@shaw.ca</t>
+  </si>
+  <si>
+    <t>Helen Kim</t>
+  </si>
+  <si>
+    <t>778-995-8949</t>
+  </si>
+  <si>
+    <t>ekhelen@gmail.com</t>
+  </si>
+  <si>
+    <t>Hez Lang</t>
+  </si>
+  <si>
+    <t>hezbob@live.ca</t>
+  </si>
+  <si>
+    <t>Maxine Ham</t>
+  </si>
+  <si>
+    <t>604-385-0557</t>
+  </si>
+  <si>
+    <t>birdiemax@shaw.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-374-6238 </t>
+  </si>
+  <si>
+    <t>Jean Kim</t>
+  </si>
+  <si>
+    <t>778-551-0332</t>
+  </si>
+  <si>
+    <t>kimjean388@gmail.com</t>
+  </si>
+  <si>
+    <t>Cynthia Lewis</t>
+  </si>
+  <si>
+    <t>clewisinc@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,12 +553,6 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -613,6 +586,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -622,7 +608,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -688,12 +674,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -702,19 +716,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -738,15 +760,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>419099</xdr:colOff>
+      <xdr:colOff>57149</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1142998</xdr:colOff>
+      <xdr:colOff>781048</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>809624</xdr:rowOff>
+      <xdr:rowOff>790574</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -775,7 +797,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="419099" y="85725"/>
+          <a:off x="57149" y="66675"/>
           <a:ext cx="723899" cy="723899"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -827,6 +849,56 @@
         <a:xfrm>
           <a:off x="4661815" y="114300"/>
           <a:ext cx="1091616" cy="714592"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1047749</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>247105</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2352674</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>657224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6695C4C-3330-4B1B-94E8-6E9E8E1F68D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1047749" y="247105"/>
+          <a:ext cx="1304925" cy="410119"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1135,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0712AD7A-AF80-42A2-A77A-ABE881FA3602}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,28 +1218,28 @@
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="14"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>40</v>
+      <c r="A2" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1184,159 +1256,157 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>7</v>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>11</v>
+      <c r="A5" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>15</v>
+      <c r="A6" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>31</v>
+      <c r="A7" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>157</v>
+      <c r="A13" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>89</v>
+      <c r="A15" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1344,513 +1414,487 @@
         <v>0</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="B42" s="8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="C42" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="D42" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>43</v>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>136</v>
+      <c r="B49" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D54" s="11" t="s">
-        <v>169</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1859,56 +1903,55 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{CAB076E5-5769-425E-887C-17C75E09CDF8}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{EE0BB6DA-6BD4-4F51-9CB3-34C0E6C83F92}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{97F3454C-E70C-48B5-8BA3-232A8D8DA295}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{CB7D14C1-85F5-44CD-B70A-BCC5165C4F98}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{50254167-3D03-4942-ADCE-9A4B6B7289D1}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{0DAE04C4-5BD5-42A0-8D83-859C1CA2CDC5}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{62DF7A97-0D73-4E53-A148-9E45AAE96021}"/>
-    <hyperlink ref="D10" r:id="rId8" xr:uid="{2492B7FC-17A1-4B02-9C6D-B246A54B55B1}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{C8AFB114-3396-4455-A71E-75BFDE10E0FC}"/>
-    <hyperlink ref="D13" r:id="rId10" xr:uid="{301567D7-D210-4608-98D1-D06A2E3003D3}"/>
-    <hyperlink ref="D16" r:id="rId11" xr:uid="{A5A4ED09-7C7A-4CDF-AB77-62F14C4D2FED}"/>
-    <hyperlink ref="D17" r:id="rId12" xr:uid="{82DBF6ED-0649-4599-BBF3-E63FECECBA79}"/>
-    <hyperlink ref="D18" r:id="rId13" xr:uid="{CD919761-5F74-4CA5-AB2C-87AA494E1C34}"/>
-    <hyperlink ref="D19" r:id="rId14" xr:uid="{F58A38EA-C689-4AE5-8120-078BECBEA04E}"/>
-    <hyperlink ref="D20" r:id="rId15" xr:uid="{3A9B3972-6FBB-4B2D-96D6-B1D3896F09A1}"/>
-    <hyperlink ref="D21" r:id="rId16" xr:uid="{DD2D3C2E-C1F0-47B0-B248-B52ED840918E}"/>
-    <hyperlink ref="D22" r:id="rId17" xr:uid="{1BB5B180-8DCD-4BEA-B39E-2A9374C44CEB}"/>
-    <hyperlink ref="D24" r:id="rId18" xr:uid="{8D5DEDF2-59D0-42BE-B38A-1B2E21C406D2}"/>
-    <hyperlink ref="D25" r:id="rId19" xr:uid="{099B24D7-0E5B-477D-B007-9EF23FD45960}"/>
-    <hyperlink ref="D26" r:id="rId20" xr:uid="{562A97F9-FBE1-46A8-9B69-762593EEF289}"/>
-    <hyperlink ref="D27" r:id="rId21" xr:uid="{15A46AF6-CE9D-4D6D-8A96-C63CD3E4D513}"/>
-    <hyperlink ref="D28" r:id="rId22" xr:uid="{DE3FB88C-EC91-47BD-9E51-536B34B31C30}"/>
-    <hyperlink ref="D30" r:id="rId23" xr:uid="{10FCAC3F-4588-4281-9BD4-FA62304B63D1}"/>
-    <hyperlink ref="D12" r:id="rId24" xr:uid="{7021A7BE-7826-424C-B09A-15DCBC35FF14}"/>
-    <hyperlink ref="D29" r:id="rId25" xr:uid="{11E9055D-4AB6-40D8-B920-7D5F95D0A772}"/>
-    <hyperlink ref="D46" r:id="rId26" xr:uid="{E1AFFE69-3CF4-4D85-A787-EF59DD0E4ADF}"/>
-    <hyperlink ref="D33" r:id="rId27" xr:uid="{384FF9DA-8B97-472E-8F6E-DEC133089AF9}"/>
-    <hyperlink ref="D34" r:id="rId28" xr:uid="{C3C6E4AD-AC1C-4C74-A002-A9FD29508A62}"/>
-    <hyperlink ref="D35" r:id="rId29" xr:uid="{A3E629D2-6DEF-4A1F-8409-15B67EEC5379}"/>
-    <hyperlink ref="D36" r:id="rId30" xr:uid="{56D4D6C0-90F9-4452-9314-2A1A83684AAC}"/>
-    <hyperlink ref="D37" r:id="rId31" xr:uid="{4A2D84E9-59B8-459A-842B-57D42A1024D7}"/>
-    <hyperlink ref="D38" r:id="rId32" xr:uid="{E31DCC33-A34A-4B55-B270-D213E3D36599}"/>
-    <hyperlink ref="D39" r:id="rId33" xr:uid="{5DAA6E02-845D-48C8-ACB2-445923702F13}"/>
-    <hyperlink ref="D40" r:id="rId34" xr:uid="{CEBD703B-9EF6-4C0A-84B1-A841B1C46779}"/>
-    <hyperlink ref="D41" r:id="rId35" xr:uid="{BA771A9D-75A0-4223-901A-D27DAF65D2FB}"/>
-    <hyperlink ref="D42" r:id="rId36" xr:uid="{8462EC55-1679-4BED-A932-72C08043FD57}"/>
-    <hyperlink ref="D43" r:id="rId37" xr:uid="{CA567127-C9C0-400D-A13E-C6E36954FD2B}"/>
-    <hyperlink ref="D44" r:id="rId38" xr:uid="{F0A07242-628E-434A-BC38-06822158A19C}"/>
-    <hyperlink ref="D45" r:id="rId39" xr:uid="{7BAFF492-0E61-491E-8AEA-7435AA32D6C3}"/>
-    <hyperlink ref="D49" r:id="rId40" xr:uid="{19D20530-C588-4955-8B0E-6317AD126FD0}"/>
-    <hyperlink ref="D50" r:id="rId41" xr:uid="{F3C2D34C-2F30-48DC-B80C-04BB42082881}"/>
-    <hyperlink ref="D51" r:id="rId42" xr:uid="{EDFB3AA0-4FA7-4A30-8945-EF054405DE58}"/>
-    <hyperlink ref="D52" r:id="rId43" xr:uid="{C3190156-A84F-4969-ADC9-48285549485D}"/>
-    <hyperlink ref="D54" r:id="rId44" xr:uid="{079C66A5-AB96-47DA-9A9E-E24CDA00713E}"/>
-    <hyperlink ref="D53" r:id="rId45" xr:uid="{7AD2AEB1-0A9D-41CD-A812-FB3D503FAE44}"/>
+    <hyperlink ref="D11" r:id="rId2" xr:uid="{2492B7FC-17A1-4B02-9C6D-B246A54B55B1}"/>
+    <hyperlink ref="D13" r:id="rId3" xr:uid="{301567D7-D210-4608-98D1-D06A2E3003D3}"/>
+    <hyperlink ref="D16" r:id="rId4" xr:uid="{A5A4ED09-7C7A-4CDF-AB77-62F14C4D2FED}"/>
+    <hyperlink ref="D17" r:id="rId5" xr:uid="{82DBF6ED-0649-4599-BBF3-E63FECECBA79}"/>
+    <hyperlink ref="D18" r:id="rId6" xr:uid="{CD919761-5F74-4CA5-AB2C-87AA494E1C34}"/>
+    <hyperlink ref="D19" r:id="rId7" xr:uid="{F58A38EA-C689-4AE5-8120-078BECBEA04E}"/>
+    <hyperlink ref="D20" r:id="rId8" xr:uid="{3A9B3972-6FBB-4B2D-96D6-B1D3896F09A1}"/>
+    <hyperlink ref="D21" r:id="rId9" xr:uid="{DD2D3C2E-C1F0-47B0-B248-B52ED840918E}"/>
+    <hyperlink ref="D22" r:id="rId10" xr:uid="{562A97F9-FBE1-46A8-9B69-762593EEF289}"/>
+    <hyperlink ref="D23" r:id="rId11" xr:uid="{15A46AF6-CE9D-4D6D-8A96-C63CD3E4D513}"/>
+    <hyperlink ref="D25" r:id="rId12" xr:uid="{10FCAC3F-4588-4281-9BD4-FA62304B63D1}"/>
+    <hyperlink ref="D12" r:id="rId13" xr:uid="{7021A7BE-7826-424C-B09A-15DCBC35FF14}"/>
+    <hyperlink ref="D24" r:id="rId14" xr:uid="{11E9055D-4AB6-40D8-B920-7D5F95D0A772}"/>
+    <hyperlink ref="D42" r:id="rId15" xr:uid="{E1AFFE69-3CF4-4D85-A787-EF59DD0E4ADF}"/>
+    <hyperlink ref="D28" r:id="rId16" xr:uid="{384FF9DA-8B97-472E-8F6E-DEC133089AF9}"/>
+    <hyperlink ref="D29" r:id="rId17" xr:uid="{C3C6E4AD-AC1C-4C74-A002-A9FD29508A62}"/>
+    <hyperlink ref="D30" r:id="rId18" xr:uid="{A3E629D2-6DEF-4A1F-8409-15B67EEC5379}"/>
+    <hyperlink ref="D31" r:id="rId19" xr:uid="{56D4D6C0-90F9-4452-9314-2A1A83684AAC}"/>
+    <hyperlink ref="D32" r:id="rId20" xr:uid="{4A2D84E9-59B8-459A-842B-57D42A1024D7}"/>
+    <hyperlink ref="D33" r:id="rId21" xr:uid="{E31DCC33-A34A-4B55-B270-D213E3D36599}"/>
+    <hyperlink ref="D34" r:id="rId22" xr:uid="{5DAA6E02-845D-48C8-ACB2-445923702F13}"/>
+    <hyperlink ref="D35" r:id="rId23" xr:uid="{CEBD703B-9EF6-4C0A-84B1-A841B1C46779}"/>
+    <hyperlink ref="D38" r:id="rId24" xr:uid="{BA771A9D-75A0-4223-901A-D27DAF65D2FB}"/>
+    <hyperlink ref="D37" r:id="rId25" xr:uid="{8462EC55-1679-4BED-A932-72C08043FD57}"/>
+    <hyperlink ref="D39" r:id="rId26" xr:uid="{F0A07242-628E-434A-BC38-06822158A19C}"/>
+    <hyperlink ref="D40" r:id="rId27" xr:uid="{7BAFF492-0E61-491E-8AEA-7435AA32D6C3}"/>
+    <hyperlink ref="D45" r:id="rId28" xr:uid="{19D20530-C588-4955-8B0E-6317AD126FD0}"/>
+    <hyperlink ref="D46" r:id="rId29" xr:uid="{F3C2D34C-2F30-48DC-B80C-04BB42082881}"/>
+    <hyperlink ref="D47" r:id="rId30" xr:uid="{EDFB3AA0-4FA7-4A30-8945-EF054405DE58}"/>
+    <hyperlink ref="D50" r:id="rId31" xr:uid="{C3190156-A84F-4969-ADC9-48285549485D}"/>
+    <hyperlink ref="D52" r:id="rId32" xr:uid="{079C66A5-AB96-47DA-9A9E-E24CDA00713E}"/>
+    <hyperlink ref="D51" r:id="rId33" xr:uid="{7AD2AEB1-0A9D-41CD-A812-FB3D503FAE44}"/>
+    <hyperlink ref="D36" r:id="rId34" xr:uid="{C9092A6A-F7E1-448C-AAD0-2921A0575687}"/>
+    <hyperlink ref="D48" r:id="rId35" xr:uid="{693DA724-A234-42E9-943F-AB9254158023}"/>
+    <hyperlink ref="D49" r:id="rId36" xr:uid="{2972100D-C4AB-42D2-AC3E-B5D901A1093F}"/>
+    <hyperlink ref="D8" r:id="rId37" xr:uid="{D6CE668D-B7ED-440F-A1B5-E6B38F8CC6F6}"/>
+    <hyperlink ref="D9" r:id="rId38" xr:uid="{B18E2662-EC36-4B93-A3C8-F0C331667EB3}"/>
+    <hyperlink ref="D10" r:id="rId39" tooltip="mailto:kimjean388@gmail.com" xr:uid="{1860DC07-B915-40AD-A963-1B410B6504A2}"/>
+    <hyperlink ref="D6" r:id="rId40" xr:uid="{35475D8D-0F9F-4B1A-95AA-87275A65EDBD}"/>
+    <hyperlink ref="D4" r:id="rId41" tooltip="mailto:ddweden@gmail.com" xr:uid="{A9DD084F-FC95-4EA1-B4BE-24E536CD0F4D}"/>
+    <hyperlink ref="D7" r:id="rId42" xr:uid="{995504E5-D2F9-4110-9F93-9537446A7808}"/>
+    <hyperlink ref="D5" r:id="rId43" xr:uid="{54F9E840-B926-4205-B8A1-F3C627FA102D}"/>
+    <hyperlink ref="D41" r:id="rId44" xr:uid="{76F93F9D-29DB-4922-B45B-8E2F3E8219F7}"/>
   </hyperlinks>
   <pageMargins left="1.2" right="0.45" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup scale="94" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId46"/>
+  <pageSetup scale="94" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId45"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="31" max="3" man="1"/>
+    <brk id="26" max="3" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId47"/>
+  <drawing r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SW modified team 3 captains
</commit_message>
<xml_diff>
--- a/secure/team-captains-list2019.xlsx
+++ b/secure/team-captains-list2019.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC18D8A4-5D91-4702-8799-4681572A7EB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DA3B7F-E9A1-4A21-A062-B3502ED4C3AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1935" windowWidth="21540" windowHeight="14265" xr2:uid="{A3301E8E-CBA9-48DE-A787-1B2E0D3F0D20}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21540" windowHeight="14265" xr2:uid="{A3301E8E-CBA9-48DE-A787-1B2E0D3F0D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$54</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="168">
   <si>
     <t>Burnaby Mountain</t>
   </si>
@@ -193,9 +193,6 @@
     <t>lisa.avery.slp@gmail.com</t>
   </si>
   <si>
-    <t>Marion Logan</t>
-  </si>
-  <si>
     <t>604-544-4231</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>Delta</t>
   </si>
   <si>
-    <t>Marilyn O'Keefe</t>
-  </si>
-  <si>
     <t>778-291-0416</t>
   </si>
   <si>
@@ -253,15 +247,6 @@
     <t>bougielinda@gmail.com</t>
   </si>
   <si>
-    <t>Anne Findlay-Shirras</t>
-  </si>
-  <si>
-    <t>604-736-9090</t>
-  </si>
-  <si>
-    <t>annefindlayshirras@gmail.com</t>
-  </si>
-  <si>
     <t>Mylora Thursday</t>
   </si>
   <si>
@@ -521,6 +506,33 @@
   </si>
   <si>
     <t>clewisinc@gmail.com</t>
+  </si>
+  <si>
+    <t>Theresa Choi (co-chair)</t>
+  </si>
+  <si>
+    <t>Marion Logan (co-chair)</t>
+  </si>
+  <si>
+    <t>theresachoi@shaw.ca</t>
+  </si>
+  <si>
+    <t>Daryl Pare (co-chair)</t>
+  </si>
+  <si>
+    <t>Cheri Hallgrimson (co-chair)</t>
+  </si>
+  <si>
+    <t>604-589-9435</t>
+  </si>
+  <si>
+    <t>chetom1@telus.net</t>
+  </si>
+  <si>
+    <t>Judy Sewell</t>
+  </si>
+  <si>
+    <t>judysewell@shaw.ca</t>
   </si>
 </sst>
 </file>
@@ -608,7 +620,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -675,12 +687,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -693,11 +703,61 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -707,7 +767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -722,21 +782,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1207,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0712AD7A-AF80-42A2-A77A-ABE881FA3602}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,18 +1288,18 @@
     <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="13"/>
+      <c r="B1" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1238,12 +1308,12 @@
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1257,103 +1327,103 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="B9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="20" t="s">
+      <c r="B10" s="3" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="C10" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="D10" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1367,7 +1437,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1381,17 +1451,17 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>111</v>
+      <c r="A13" s="24" t="s">
+        <v>106</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1405,7 +1475,7 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1537,22 +1607,22 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1560,7 +1630,7 @@
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1579,327 +1649,343 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="6" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="B31" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D31" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="6" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="B32" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="D32" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
       <c r="B33" s="3" t="s">
-        <v>68</v>
+        <v>163</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>135</v>
+        <v>27</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>136</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>137</v>
+        <v>70</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>83</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C37" s="3"/>
       <c r="D37" s="6" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B47" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C47" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D47" s="5" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="D48" s="6" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C53" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D53" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>126</v>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{CAB076E5-5769-425E-887C-17C75E09CDF8}"/>
@@ -1916,42 +2002,43 @@
     <hyperlink ref="D25" r:id="rId12" xr:uid="{10FCAC3F-4588-4281-9BD4-FA62304B63D1}"/>
     <hyperlink ref="D12" r:id="rId13" xr:uid="{7021A7BE-7826-424C-B09A-15DCBC35FF14}"/>
     <hyperlink ref="D24" r:id="rId14" xr:uid="{11E9055D-4AB6-40D8-B920-7D5F95D0A772}"/>
-    <hyperlink ref="D42" r:id="rId15" xr:uid="{E1AFFE69-3CF4-4D85-A787-EF59DD0E4ADF}"/>
+    <hyperlink ref="D44" r:id="rId15" xr:uid="{E1AFFE69-3CF4-4D85-A787-EF59DD0E4ADF}"/>
     <hyperlink ref="D28" r:id="rId16" xr:uid="{384FF9DA-8B97-472E-8F6E-DEC133089AF9}"/>
     <hyperlink ref="D29" r:id="rId17" xr:uid="{C3C6E4AD-AC1C-4C74-A002-A9FD29508A62}"/>
-    <hyperlink ref="D30" r:id="rId18" xr:uid="{A3E629D2-6DEF-4A1F-8409-15B67EEC5379}"/>
-    <hyperlink ref="D31" r:id="rId19" xr:uid="{56D4D6C0-90F9-4452-9314-2A1A83684AAC}"/>
-    <hyperlink ref="D32" r:id="rId20" xr:uid="{4A2D84E9-59B8-459A-842B-57D42A1024D7}"/>
-    <hyperlink ref="D33" r:id="rId21" xr:uid="{E31DCC33-A34A-4B55-B270-D213E3D36599}"/>
-    <hyperlink ref="D34" r:id="rId22" xr:uid="{5DAA6E02-845D-48C8-ACB2-445923702F13}"/>
-    <hyperlink ref="D35" r:id="rId23" xr:uid="{CEBD703B-9EF6-4C0A-84B1-A841B1C46779}"/>
-    <hyperlink ref="D38" r:id="rId24" xr:uid="{BA771A9D-75A0-4223-901A-D27DAF65D2FB}"/>
-    <hyperlink ref="D37" r:id="rId25" xr:uid="{8462EC55-1679-4BED-A932-72C08043FD57}"/>
-    <hyperlink ref="D39" r:id="rId26" xr:uid="{F0A07242-628E-434A-BC38-06822158A19C}"/>
-    <hyperlink ref="D40" r:id="rId27" xr:uid="{7BAFF492-0E61-491E-8AEA-7435AA32D6C3}"/>
-    <hyperlink ref="D45" r:id="rId28" xr:uid="{19D20530-C588-4955-8B0E-6317AD126FD0}"/>
-    <hyperlink ref="D46" r:id="rId29" xr:uid="{F3C2D34C-2F30-48DC-B80C-04BB42082881}"/>
-    <hyperlink ref="D47" r:id="rId30" xr:uid="{EDFB3AA0-4FA7-4A30-8945-EF054405DE58}"/>
-    <hyperlink ref="D50" r:id="rId31" xr:uid="{C3190156-A84F-4969-ADC9-48285549485D}"/>
-    <hyperlink ref="D52" r:id="rId32" xr:uid="{079C66A5-AB96-47DA-9A9E-E24CDA00713E}"/>
-    <hyperlink ref="D51" r:id="rId33" xr:uid="{7AD2AEB1-0A9D-41CD-A812-FB3D503FAE44}"/>
-    <hyperlink ref="D36" r:id="rId34" xr:uid="{C9092A6A-F7E1-448C-AAD0-2921A0575687}"/>
-    <hyperlink ref="D48" r:id="rId35" xr:uid="{693DA724-A234-42E9-943F-AB9254158023}"/>
-    <hyperlink ref="D49" r:id="rId36" xr:uid="{2972100D-C4AB-42D2-AC3E-B5D901A1093F}"/>
-    <hyperlink ref="D8" r:id="rId37" xr:uid="{D6CE668D-B7ED-440F-A1B5-E6B38F8CC6F6}"/>
-    <hyperlink ref="D9" r:id="rId38" xr:uid="{B18E2662-EC36-4B93-A3C8-F0C331667EB3}"/>
-    <hyperlink ref="D10" r:id="rId39" tooltip="mailto:kimjean388@gmail.com" xr:uid="{1860DC07-B915-40AD-A963-1B410B6504A2}"/>
-    <hyperlink ref="D6" r:id="rId40" xr:uid="{35475D8D-0F9F-4B1A-95AA-87275A65EDBD}"/>
-    <hyperlink ref="D4" r:id="rId41" tooltip="mailto:ddweden@gmail.com" xr:uid="{A9DD084F-FC95-4EA1-B4BE-24E536CD0F4D}"/>
-    <hyperlink ref="D7" r:id="rId42" xr:uid="{995504E5-D2F9-4110-9F93-9537446A7808}"/>
-    <hyperlink ref="D5" r:id="rId43" xr:uid="{54F9E840-B926-4205-B8A1-F3C627FA102D}"/>
-    <hyperlink ref="D41" r:id="rId44" xr:uid="{76F93F9D-29DB-4922-B45B-8E2F3E8219F7}"/>
+    <hyperlink ref="D31" r:id="rId18" xr:uid="{A3E629D2-6DEF-4A1F-8409-15B67EEC5379}"/>
+    <hyperlink ref="D32" r:id="rId19" xr:uid="{56D4D6C0-90F9-4452-9314-2A1A83684AAC}"/>
+    <hyperlink ref="D34" r:id="rId20" xr:uid="{4A2D84E9-59B8-459A-842B-57D42A1024D7}"/>
+    <hyperlink ref="D35" r:id="rId21" xr:uid="{E31DCC33-A34A-4B55-B270-D213E3D36599}"/>
+    <hyperlink ref="D36" r:id="rId22" xr:uid="{5DAA6E02-845D-48C8-ACB2-445923702F13}"/>
+    <hyperlink ref="D37" r:id="rId23" xr:uid="{CEBD703B-9EF6-4C0A-84B1-A841B1C46779}"/>
+    <hyperlink ref="D40" r:id="rId24" xr:uid="{BA771A9D-75A0-4223-901A-D27DAF65D2FB}"/>
+    <hyperlink ref="D39" r:id="rId25" xr:uid="{8462EC55-1679-4BED-A932-72C08043FD57}"/>
+    <hyperlink ref="D42" r:id="rId26" xr:uid="{7BAFF492-0E61-491E-8AEA-7435AA32D6C3}"/>
+    <hyperlink ref="D47" r:id="rId27" xr:uid="{19D20530-C588-4955-8B0E-6317AD126FD0}"/>
+    <hyperlink ref="D48" r:id="rId28" xr:uid="{F3C2D34C-2F30-48DC-B80C-04BB42082881}"/>
+    <hyperlink ref="D49" r:id="rId29" xr:uid="{EDFB3AA0-4FA7-4A30-8945-EF054405DE58}"/>
+    <hyperlink ref="D52" r:id="rId30" xr:uid="{C3190156-A84F-4969-ADC9-48285549485D}"/>
+    <hyperlink ref="D54" r:id="rId31" xr:uid="{079C66A5-AB96-47DA-9A9E-E24CDA00713E}"/>
+    <hyperlink ref="D53" r:id="rId32" xr:uid="{7AD2AEB1-0A9D-41CD-A812-FB3D503FAE44}"/>
+    <hyperlink ref="D38" r:id="rId33" xr:uid="{C9092A6A-F7E1-448C-AAD0-2921A0575687}"/>
+    <hyperlink ref="D50" r:id="rId34" xr:uid="{693DA724-A234-42E9-943F-AB9254158023}"/>
+    <hyperlink ref="D51" r:id="rId35" xr:uid="{2972100D-C4AB-42D2-AC3E-B5D901A1093F}"/>
+    <hyperlink ref="D8" r:id="rId36" xr:uid="{D6CE668D-B7ED-440F-A1B5-E6B38F8CC6F6}"/>
+    <hyperlink ref="D9" r:id="rId37" xr:uid="{B18E2662-EC36-4B93-A3C8-F0C331667EB3}"/>
+    <hyperlink ref="D10" r:id="rId38" tooltip="mailto:kimjean388@gmail.com" xr:uid="{1860DC07-B915-40AD-A963-1B410B6504A2}"/>
+    <hyperlink ref="D6" r:id="rId39" xr:uid="{35475D8D-0F9F-4B1A-95AA-87275A65EDBD}"/>
+    <hyperlink ref="D4" r:id="rId40" tooltip="mailto:ddweden@gmail.com" xr:uid="{A9DD084F-FC95-4EA1-B4BE-24E536CD0F4D}"/>
+    <hyperlink ref="D7" r:id="rId41" xr:uid="{995504E5-D2F9-4110-9F93-9537446A7808}"/>
+    <hyperlink ref="D5" r:id="rId42" xr:uid="{54F9E840-B926-4205-B8A1-F3C627FA102D}"/>
+    <hyperlink ref="D43" r:id="rId43" xr:uid="{76F93F9D-29DB-4922-B45B-8E2F3E8219F7}"/>
+    <hyperlink ref="D30" r:id="rId44" xr:uid="{72DD4FB5-0D0D-4DC1-8099-35C3B012CC11}"/>
+    <hyperlink ref="D33" r:id="rId45" xr:uid="{11C0EF3F-D0E5-4FCD-8255-6E4489A603B6}"/>
   </hyperlinks>
   <pageMargins left="1.2" right="0.45" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup scale="94" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId45"/>
+  <pageSetup scale="94" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId46"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="26" max="3" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId46"/>
+  <drawing r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SW modified team 2 contacts:
</commit_message>
<xml_diff>
--- a/secure/team-captains-list2019.xlsx
+++ b/secure/team-captains-list2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DA3B7F-E9A1-4A21-A062-B3502ED4C3AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C45A170-6B45-4E2D-8A29-388C1D02E7E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21540" windowHeight="14265" xr2:uid="{A3301E8E-CBA9-48DE-A787-1B2E0D3F0D20}"/>
+    <workbookView xWindow="2400" yWindow="240" windowWidth="21540" windowHeight="14265" xr2:uid="{A3301E8E-CBA9-48DE-A787-1B2E0D3F0D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="168">
   <si>
     <t>Burnaby Mountain</t>
   </si>
@@ -91,15 +91,6 @@
     <t>Fraserview</t>
   </si>
   <si>
-    <t>Julie Winton</t>
-  </si>
-  <si>
-    <t>604-736-6893</t>
-  </si>
-  <si>
-    <t>jwinton2211@gmail.com</t>
-  </si>
-  <si>
     <t>Greenacres</t>
   </si>
   <si>
@@ -533,6 +524,15 @@
   </si>
   <si>
     <t>judysewell@shaw.ca</t>
+  </si>
+  <si>
+    <t>Cindi Ee</t>
+  </si>
+  <si>
+    <t>604-830-7760</t>
+  </si>
+  <si>
+    <t>cindi0516@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -767,7 +767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -785,6 +785,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -797,16 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1280,7 +1281,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,13 +1294,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
-      <c r="B1" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C1" s="16"/>
+      <c r="B1" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1313,7 +1314,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1328,98 +1329,98 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>141</v>
+        <v>136</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>152</v>
+        <v>148</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>138</v>
+        <v>150</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>156</v>
+        <v>152</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1437,7 +1438,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1451,23 +1452,23 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
@@ -1498,83 +1499,83 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>165</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>22</v>
+        <v>166</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1582,13 +1583,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1596,33 +1597,33 @@
         <v>8</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1636,80 +1637,80 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D29" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="3" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="B32" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="3" t="s">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1717,100 +1718,100 @@
         <v>19</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1818,48 +1819,48 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20" t="s">
-        <v>158</v>
+      <c r="B43" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="16" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>13</v>
@@ -1873,112 +1874,112 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" s="10" t="s">
         <v>118</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SW modified team 3 contact
</commit_message>
<xml_diff>
--- a/secure/team-captains-list2019.xlsx
+++ b/secure/team-captains-list2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shwor\Desktop\BCG-Zone-4\secure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C45A170-6B45-4E2D-8A29-388C1D02E7E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{74D15CAA-A644-48D3-88EE-2AAEF087A195}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="240" windowWidth="21540" windowHeight="14265" xr2:uid="{A3301E8E-CBA9-48DE-A787-1B2E0D3F0D20}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21540" windowHeight="14265" xr2:uid="{A3301E8E-CBA9-48DE-A787-1B2E0D3F0D20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="172">
   <si>
     <t>Burnaby Mountain</t>
   </si>
@@ -520,12 +520,6 @@
     <t>chetom1@telus.net</t>
   </si>
   <si>
-    <t>Judy Sewell</t>
-  </si>
-  <si>
-    <t>judysewell@shaw.ca</t>
-  </si>
-  <si>
     <t>Cindi Ee</t>
   </si>
   <si>
@@ -533,13 +527,31 @@
   </si>
   <si>
     <t>cindi0516@gmail.com</t>
+  </si>
+  <si>
+    <t>Mairi Blair</t>
+  </si>
+  <si>
+    <t>604-505-1249</t>
+  </si>
+  <si>
+    <t>bla8873@telus.net</t>
+  </si>
+  <si>
+    <t>Anne Findlay-Shirras</t>
+  </si>
+  <si>
+    <t>604-736-9090</t>
+  </si>
+  <si>
+    <t>annefindlayshirras@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -611,6 +623,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -620,7 +640,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -762,12 +782,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -786,7 +880,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -807,7 +900,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1281,7 +1379,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A54" sqref="A1:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,13 +1392,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1314,7 +1412,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1334,10 +1432,10 @@
       <c r="B4" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1391,7 +1489,7 @@
       <c r="C8" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1405,7 +1503,7 @@
       <c r="C9" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1419,7 +1517,7 @@
       <c r="C10" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="21" t="s">
         <v>153</v>
       </c>
     </row>
@@ -1438,7 +1536,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1452,7 +1550,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>103</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1499,13 +1597,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1631,7 +1729,7 @@
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1645,12 +1743,12 @@
       <c r="C28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="27" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1659,17 +1757,17 @@
       <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="28" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1683,12 +1781,12 @@
       <c r="C31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="28" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="24" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -1697,19 +1795,19 @@
       <c r="C32" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="28" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="3" t="s">
         <v>160</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="28" t="s">
         <v>162</v>
       </c>
     </row>
@@ -1723,7 +1821,7 @@
       <c r="C34" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="28" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1737,7 +1835,7 @@
       <c r="C35" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="28" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1751,7 +1849,7 @@
       <c r="C36" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="28" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1760,11 +1858,13 @@
         <v>28</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="6" t="s">
-        <v>164</v>
+        <v>169</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1777,7 +1877,7 @@
       <c r="C38" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="28" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1791,7 +1891,7 @@
       <c r="C39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="28" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1805,7 +1905,7 @@
       <c r="C40" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="28" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1813,9 +1913,15 @@
       <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="6"/>
+      <c r="B41" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -1827,7 +1933,7 @@
       <c r="C42" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="28" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1839,7 +1945,7 @@
         <v>154</v>
       </c>
       <c r="C43" s="15"/>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="29" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1853,7 +1959,7 @@
       <c r="C44" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="30" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2011,29 +2117,29 @@
     <hyperlink ref="D34" r:id="rId20" xr:uid="{4A2D84E9-59B8-459A-842B-57D42A1024D7}"/>
     <hyperlink ref="D35" r:id="rId21" xr:uid="{E31DCC33-A34A-4B55-B270-D213E3D36599}"/>
     <hyperlink ref="D36" r:id="rId22" xr:uid="{5DAA6E02-845D-48C8-ACB2-445923702F13}"/>
-    <hyperlink ref="D37" r:id="rId23" xr:uid="{CEBD703B-9EF6-4C0A-84B1-A841B1C46779}"/>
-    <hyperlink ref="D40" r:id="rId24" xr:uid="{BA771A9D-75A0-4223-901A-D27DAF65D2FB}"/>
-    <hyperlink ref="D39" r:id="rId25" xr:uid="{8462EC55-1679-4BED-A932-72C08043FD57}"/>
-    <hyperlink ref="D42" r:id="rId26" xr:uid="{7BAFF492-0E61-491E-8AEA-7435AA32D6C3}"/>
-    <hyperlink ref="D47" r:id="rId27" xr:uid="{19D20530-C588-4955-8B0E-6317AD126FD0}"/>
-    <hyperlink ref="D48" r:id="rId28" xr:uid="{F3C2D34C-2F30-48DC-B80C-04BB42082881}"/>
-    <hyperlink ref="D49" r:id="rId29" xr:uid="{EDFB3AA0-4FA7-4A30-8945-EF054405DE58}"/>
-    <hyperlink ref="D52" r:id="rId30" xr:uid="{C3190156-A84F-4969-ADC9-48285549485D}"/>
-    <hyperlink ref="D54" r:id="rId31" xr:uid="{079C66A5-AB96-47DA-9A9E-E24CDA00713E}"/>
-    <hyperlink ref="D53" r:id="rId32" xr:uid="{7AD2AEB1-0A9D-41CD-A812-FB3D503FAE44}"/>
-    <hyperlink ref="D38" r:id="rId33" xr:uid="{C9092A6A-F7E1-448C-AAD0-2921A0575687}"/>
-    <hyperlink ref="D50" r:id="rId34" xr:uid="{693DA724-A234-42E9-943F-AB9254158023}"/>
-    <hyperlink ref="D51" r:id="rId35" xr:uid="{2972100D-C4AB-42D2-AC3E-B5D901A1093F}"/>
-    <hyperlink ref="D8" r:id="rId36" xr:uid="{D6CE668D-B7ED-440F-A1B5-E6B38F8CC6F6}"/>
-    <hyperlink ref="D9" r:id="rId37" xr:uid="{B18E2662-EC36-4B93-A3C8-F0C331667EB3}"/>
-    <hyperlink ref="D10" r:id="rId38" tooltip="mailto:kimjean388@gmail.com" xr:uid="{1860DC07-B915-40AD-A963-1B410B6504A2}"/>
-    <hyperlink ref="D6" r:id="rId39" xr:uid="{35475D8D-0F9F-4B1A-95AA-87275A65EDBD}"/>
-    <hyperlink ref="D4" r:id="rId40" tooltip="mailto:ddweden@gmail.com" xr:uid="{A9DD084F-FC95-4EA1-B4BE-24E536CD0F4D}"/>
-    <hyperlink ref="D7" r:id="rId41" xr:uid="{995504E5-D2F9-4110-9F93-9537446A7808}"/>
-    <hyperlink ref="D5" r:id="rId42" xr:uid="{54F9E840-B926-4205-B8A1-F3C627FA102D}"/>
-    <hyperlink ref="D43" r:id="rId43" xr:uid="{76F93F9D-29DB-4922-B45B-8E2F3E8219F7}"/>
-    <hyperlink ref="D30" r:id="rId44" xr:uid="{72DD4FB5-0D0D-4DC1-8099-35C3B012CC11}"/>
-    <hyperlink ref="D33" r:id="rId45" xr:uid="{11C0EF3F-D0E5-4FCD-8255-6E4489A603B6}"/>
+    <hyperlink ref="D40" r:id="rId23" xr:uid="{BA771A9D-75A0-4223-901A-D27DAF65D2FB}"/>
+    <hyperlink ref="D39" r:id="rId24" xr:uid="{8462EC55-1679-4BED-A932-72C08043FD57}"/>
+    <hyperlink ref="D42" r:id="rId25" xr:uid="{7BAFF492-0E61-491E-8AEA-7435AA32D6C3}"/>
+    <hyperlink ref="D47" r:id="rId26" xr:uid="{19D20530-C588-4955-8B0E-6317AD126FD0}"/>
+    <hyperlink ref="D48" r:id="rId27" xr:uid="{F3C2D34C-2F30-48DC-B80C-04BB42082881}"/>
+    <hyperlink ref="D49" r:id="rId28" xr:uid="{EDFB3AA0-4FA7-4A30-8945-EF054405DE58}"/>
+    <hyperlink ref="D52" r:id="rId29" xr:uid="{C3190156-A84F-4969-ADC9-48285549485D}"/>
+    <hyperlink ref="D54" r:id="rId30" xr:uid="{079C66A5-AB96-47DA-9A9E-E24CDA00713E}"/>
+    <hyperlink ref="D53" r:id="rId31" xr:uid="{7AD2AEB1-0A9D-41CD-A812-FB3D503FAE44}"/>
+    <hyperlink ref="D38" r:id="rId32" xr:uid="{C9092A6A-F7E1-448C-AAD0-2921A0575687}"/>
+    <hyperlink ref="D50" r:id="rId33" xr:uid="{693DA724-A234-42E9-943F-AB9254158023}"/>
+    <hyperlink ref="D51" r:id="rId34" xr:uid="{2972100D-C4AB-42D2-AC3E-B5D901A1093F}"/>
+    <hyperlink ref="D8" r:id="rId35" xr:uid="{D6CE668D-B7ED-440F-A1B5-E6B38F8CC6F6}"/>
+    <hyperlink ref="D9" r:id="rId36" xr:uid="{B18E2662-EC36-4B93-A3C8-F0C331667EB3}"/>
+    <hyperlink ref="D10" r:id="rId37" tooltip="mailto:kimjean388@gmail.com" xr:uid="{1860DC07-B915-40AD-A963-1B410B6504A2}"/>
+    <hyperlink ref="D6" r:id="rId38" xr:uid="{35475D8D-0F9F-4B1A-95AA-87275A65EDBD}"/>
+    <hyperlink ref="D4" r:id="rId39" tooltip="mailto:ddweden@gmail.com" xr:uid="{A9DD084F-FC95-4EA1-B4BE-24E536CD0F4D}"/>
+    <hyperlink ref="D7" r:id="rId40" xr:uid="{995504E5-D2F9-4110-9F93-9537446A7808}"/>
+    <hyperlink ref="D5" r:id="rId41" xr:uid="{54F9E840-B926-4205-B8A1-F3C627FA102D}"/>
+    <hyperlink ref="D43" r:id="rId42" xr:uid="{76F93F9D-29DB-4922-B45B-8E2F3E8219F7}"/>
+    <hyperlink ref="D30" r:id="rId43" xr:uid="{72DD4FB5-0D0D-4DC1-8099-35C3B012CC11}"/>
+    <hyperlink ref="D33" r:id="rId44" xr:uid="{11C0EF3F-D0E5-4FCD-8255-6E4489A603B6}"/>
+    <hyperlink ref="D41" r:id="rId45" xr:uid="{B7039D17-5E1A-4F9A-BA12-A39AE2338378}"/>
   </hyperlinks>
   <pageMargins left="1.2" right="0.45" top="0.5" bottom="0.5" header="0" footer="0"/>
   <pageSetup scale="94" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId46"/>

</xml_diff>